<commit_message>
#7 F-value in table 3 for Nodule model updated
</commit_message>
<xml_diff>
--- a/figures_tables/tables/table_2_fvalues.xlsx
+++ b/figures_tables/tables/table_2_fvalues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecamo19/Documents/projects/nutrients_and_water_effects_2022/stats/figures_tables/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16F5EB-95C9-AC45-986D-C30CA1ED9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92857894-29EC-4C4B-A4C7-ECA9204540C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{21EC3D8C-F6EC-D447-9FC5-6E3B8A0C7CB0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Total Biomass </t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Treatment x Group </t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
     <r>
       <t>5.76</t>
     </r>
@@ -173,21 +170,6 @@
         <family val="1"/>
       </rPr>
       <t>***</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>11.33</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>**</t>
     </r>
   </si>
   <si>
@@ -491,6 +473,51 @@
         <family val="1"/>
       </rPr>
       <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.87</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>66.58</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>***</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.23</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
     </r>
   </si>
 </sst>
@@ -599,7 +626,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -919,14 +946,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -950,27 +977,27 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.2">
@@ -978,13 +1005,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.2">
@@ -992,13 +1019,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.2">
@@ -1006,13 +1033,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.2">
@@ -1020,41 +1047,41 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="D10" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25" thickBot="1" x14ac:dyDescent="0.25">
@@ -1062,13 +1089,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>